<commit_message>
Final group results and cards
</commit_message>
<xml_diff>
--- a/world_cup_2018_full_results_fp.xlsx
+++ b/world_cup_2018_full_results_fp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\world-cup-2018-spreadsheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{343B6F09-F822-45E0-9AA4-F0E2B803AE14}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D28368E3-7F21-4E2C-A914-B6D5D89A4ACB}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -9338,89 +9338,29 @@
     <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -9502,29 +9442,89 @@
       <alignment horizontal="center" vertical="center"/>
       <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="25" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+      <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+      <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+      <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+      <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+      <protection hidden="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
+      <protection hidden="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -29741,9 +29741,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B1:AA130"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
-    </sheetView>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -29917,7 +29915,7 @@
         <v>0</v>
       </c>
       <c r="I8" s="98">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J8" s="75"/>
       <c r="L8" s="77" t="s">
@@ -30260,7 +30258,7 @@
       </c>
       <c r="T19" s="108">
         <f t="shared" si="2"/>
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="U19" s="108">
         <v>2</v>
@@ -30452,7 +30450,7 @@
         <v>0</v>
       </c>
       <c r="I24" s="98">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="J24" s="75"/>
       <c r="O24" s="108" t="s">
@@ -30932,7 +30930,7 @@
       </c>
       <c r="T35" s="108">
         <f t="shared" si="2"/>
-        <v>-8</v>
+        <v>-11</v>
       </c>
       <c r="U35" s="108">
         <v>18</v>
@@ -30956,7 +30954,7 @@
         <v>0</v>
       </c>
       <c r="I36" s="98">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J36" s="75"/>
       <c r="O36" s="108" t="s">
@@ -31289,7 +31287,7 @@
       </c>
       <c r="T47" s="108">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="U47" s="108">
         <v>30</v>
@@ -32740,8 +32738,8 @@
   </sheetPr>
   <dimension ref="A1:CA97"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J63" sqref="J63"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -32796,25 +32794,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:79" ht="46.5" x14ac:dyDescent="0.25">
-      <c r="A1" s="136" t="str">
+      <c r="A1" s="121" t="str">
         <f>INDEX(T,2,lang)</f>
         <v>2018 World Cup Final Tournament Schedule</v>
       </c>
-      <c r="B1" s="136"/>
-      <c r="C1" s="136"/>
-      <c r="D1" s="136"/>
-      <c r="E1" s="136"/>
-      <c r="F1" s="136"/>
-      <c r="G1" s="136"/>
-      <c r="H1" s="136"/>
-      <c r="I1" s="136"/>
-      <c r="J1" s="136"/>
-      <c r="K1" s="136"/>
-      <c r="L1" s="136"/>
-      <c r="M1" s="136"/>
-      <c r="N1" s="136"/>
-      <c r="O1" s="136"/>
-      <c r="P1" s="136"/>
+      <c r="B1" s="121"/>
+      <c r="C1" s="121"/>
+      <c r="D1" s="121"/>
+      <c r="E1" s="121"/>
+      <c r="F1" s="121"/>
+      <c r="G1" s="121"/>
+      <c r="H1" s="121"/>
+      <c r="I1" s="121"/>
+      <c r="J1" s="121"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="121"/>
+      <c r="M1" s="121"/>
+      <c r="N1" s="121"/>
+      <c r="O1" s="121"/>
+      <c r="P1" s="121"/>
       <c r="S1" s="101"/>
       <c r="T1" s="101"/>
       <c r="U1" s="101"/>
@@ -32883,11 +32881,11 @@
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
       <c r="N3" s="18"/>
-      <c r="O3" s="137" t="str">
+      <c r="O3" s="122" t="str">
         <f>"Language: " &amp; Settings!C4</f>
         <v>Language: English</v>
       </c>
-      <c r="P3" s="137"/>
+      <c r="P3" s="122"/>
       <c r="S3" s="101"/>
       <c r="T3" s="101"/>
       <c r="U3" s="101"/>
@@ -32916,43 +32914,43 @@
     </row>
     <row r="4" spans="1:79" ht="3" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="138" t="str">
+      <c r="A5" s="123" t="str">
         <f>INDEX(T,3,lang)</f>
         <v>Group Stage</v>
       </c>
-      <c r="B5" s="139"/>
-      <c r="C5" s="139"/>
-      <c r="D5" s="139"/>
-      <c r="E5" s="139"/>
-      <c r="F5" s="139"/>
-      <c r="G5" s="139"/>
-      <c r="H5" s="140"/>
-      <c r="J5" s="144" t="s">
+      <c r="B5" s="124"/>
+      <c r="C5" s="124"/>
+      <c r="D5" s="124"/>
+      <c r="E5" s="124"/>
+      <c r="F5" s="124"/>
+      <c r="G5" s="124"/>
+      <c r="H5" s="125"/>
+      <c r="J5" s="129" t="s">
         <v>2171</v>
       </c>
-      <c r="K5" s="145"/>
-      <c r="L5" s="145"/>
-      <c r="M5" s="145"/>
-      <c r="N5" s="145"/>
-      <c r="O5" s="145"/>
-      <c r="P5" s="146"/>
+      <c r="K5" s="130"/>
+      <c r="L5" s="130"/>
+      <c r="M5" s="130"/>
+      <c r="N5" s="130"/>
+      <c r="O5" s="130"/>
+      <c r="P5" s="131"/>
     </row>
     <row r="6" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="141"/>
-      <c r="B6" s="142"/>
-      <c r="C6" s="142"/>
-      <c r="D6" s="142"/>
-      <c r="E6" s="142"/>
-      <c r="F6" s="142"/>
-      <c r="G6" s="142"/>
-      <c r="H6" s="143"/>
-      <c r="J6" s="147"/>
-      <c r="K6" s="148"/>
-      <c r="L6" s="148"/>
-      <c r="M6" s="148"/>
-      <c r="N6" s="148"/>
-      <c r="O6" s="148"/>
-      <c r="P6" s="149"/>
+      <c r="A6" s="126"/>
+      <c r="B6" s="127"/>
+      <c r="C6" s="127"/>
+      <c r="D6" s="127"/>
+      <c r="E6" s="127"/>
+      <c r="F6" s="127"/>
+      <c r="G6" s="127"/>
+      <c r="H6" s="128"/>
+      <c r="J6" s="132"/>
+      <c r="K6" s="133"/>
+      <c r="L6" s="133"/>
+      <c r="M6" s="133"/>
+      <c r="N6" s="133"/>
+      <c r="O6" s="133"/>
+      <c r="P6" s="134"/>
       <c r="V6" s="101" t="s">
         <v>2172</v>
       </c>
@@ -33022,38 +33020,38 @@
       <c r="AW6" s="105" t="s">
         <v>2177</v>
       </c>
-      <c r="BB6" s="130" t="str">
+      <c r="BB6" s="115" t="str">
         <f>INDEX(T,4,lang)</f>
         <v>Round of 16</v>
       </c>
-      <c r="BC6" s="131"/>
-      <c r="BD6" s="131"/>
-      <c r="BE6" s="131"/>
-      <c r="BF6" s="132"/>
-      <c r="BI6" s="130" t="str">
+      <c r="BC6" s="116"/>
+      <c r="BD6" s="116"/>
+      <c r="BE6" s="116"/>
+      <c r="BF6" s="117"/>
+      <c r="BI6" s="115" t="str">
         <f>INDEX(T,5,lang)</f>
         <v>Quarterfinals</v>
       </c>
-      <c r="BJ6" s="131"/>
-      <c r="BK6" s="131"/>
-      <c r="BL6" s="131"/>
-      <c r="BM6" s="132"/>
-      <c r="BP6" s="130" t="str">
+      <c r="BJ6" s="116"/>
+      <c r="BK6" s="116"/>
+      <c r="BL6" s="116"/>
+      <c r="BM6" s="117"/>
+      <c r="BP6" s="115" t="str">
         <f>INDEX(T,6,lang)</f>
         <v>Semi-Finals</v>
       </c>
-      <c r="BQ6" s="131"/>
-      <c r="BR6" s="131"/>
-      <c r="BS6" s="131"/>
-      <c r="BT6" s="132"/>
-      <c r="BW6" s="130" t="str">
+      <c r="BQ6" s="116"/>
+      <c r="BR6" s="116"/>
+      <c r="BS6" s="116"/>
+      <c r="BT6" s="117"/>
+      <c r="BW6" s="115" t="str">
         <f>INDEX(T,8,lang)</f>
         <v>Final</v>
       </c>
-      <c r="BX6" s="131"/>
-      <c r="BY6" s="131"/>
-      <c r="BZ6" s="131"/>
-      <c r="CA6" s="132"/>
+      <c r="BX6" s="116"/>
+      <c r="BY6" s="116"/>
+      <c r="BZ6" s="116"/>
+      <c r="CA6" s="117"/>
     </row>
     <row r="7" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19">
@@ -33075,10 +33073,10 @@
         <f>AB8</f>
         <v>Russia</v>
       </c>
-      <c r="F7" s="150">
+      <c r="F7" s="109">
         <v>5</v>
       </c>
-      <c r="G7" s="151">
+      <c r="G7" s="110">
         <v>0</v>
       </c>
       <c r="H7" s="92" t="str">
@@ -33126,26 +33124,26 @@
       <c r="AP7" s="102" t="s">
         <v>2170</v>
       </c>
-      <c r="BB7" s="133"/>
-      <c r="BC7" s="134"/>
-      <c r="BD7" s="134"/>
-      <c r="BE7" s="134"/>
-      <c r="BF7" s="135"/>
-      <c r="BI7" s="133"/>
-      <c r="BJ7" s="134"/>
-      <c r="BK7" s="134"/>
-      <c r="BL7" s="134"/>
-      <c r="BM7" s="135"/>
-      <c r="BP7" s="133"/>
-      <c r="BQ7" s="134"/>
-      <c r="BR7" s="134"/>
-      <c r="BS7" s="134"/>
-      <c r="BT7" s="135"/>
-      <c r="BW7" s="133"/>
-      <c r="BX7" s="134"/>
-      <c r="BY7" s="134"/>
-      <c r="BZ7" s="134"/>
-      <c r="CA7" s="135"/>
+      <c r="BB7" s="118"/>
+      <c r="BC7" s="119"/>
+      <c r="BD7" s="119"/>
+      <c r="BE7" s="119"/>
+      <c r="BF7" s="120"/>
+      <c r="BI7" s="118"/>
+      <c r="BJ7" s="119"/>
+      <c r="BK7" s="119"/>
+      <c r="BL7" s="119"/>
+      <c r="BM7" s="120"/>
+      <c r="BP7" s="118"/>
+      <c r="BQ7" s="119"/>
+      <c r="BR7" s="119"/>
+      <c r="BS7" s="119"/>
+      <c r="BT7" s="120"/>
+      <c r="BW7" s="118"/>
+      <c r="BX7" s="119"/>
+      <c r="BY7" s="119"/>
+      <c r="BZ7" s="119"/>
+      <c r="CA7" s="120"/>
     </row>
     <row r="8" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="23">
@@ -33167,10 +33165,10 @@
         <f>AB10</f>
         <v>Egypt</v>
       </c>
-      <c r="F8" s="152">
-        <v>0</v>
-      </c>
-      <c r="G8" s="153">
+      <c r="F8" s="111">
+        <v>0</v>
+      </c>
+      <c r="G8" s="112">
         <v>1</v>
       </c>
       <c r="H8" s="93" t="str">
@@ -33364,10 +33362,10 @@
         <f>AB14</f>
         <v>Portugal</v>
       </c>
-      <c r="F9" s="152">
+      <c r="F9" s="111">
         <v>3</v>
       </c>
-      <c r="G9" s="153">
+      <c r="G9" s="112">
         <v>3</v>
       </c>
       <c r="H9" s="93" t="str">
@@ -33576,10 +33574,10 @@
         <f>AB16</f>
         <v>Morocco</v>
       </c>
-      <c r="F10" s="152">
-        <v>0</v>
-      </c>
-      <c r="G10" s="153">
+      <c r="F10" s="111">
+        <v>0</v>
+      </c>
+      <c r="G10" s="112">
         <v>1</v>
       </c>
       <c r="H10" s="93" t="str">
@@ -33734,7 +33732,7 @@
         <f>AU10-AV10</f>
         <v>0</v>
       </c>
-      <c r="BB10" s="118">
+      <c r="BB10" s="135">
         <v>49</v>
       </c>
       <c r="BC10" s="30" t="str">
@@ -33786,10 +33784,10 @@
         <f>AB20</f>
         <v>France</v>
       </c>
-      <c r="F11" s="152">
+      <c r="F11" s="111">
         <v>2</v>
       </c>
-      <c r="G11" s="153">
+      <c r="G11" s="112">
         <v>1</v>
       </c>
       <c r="H11" s="93" t="str">
@@ -33944,7 +33942,7 @@
         <f>AU11-AV11</f>
         <v>0</v>
       </c>
-      <c r="BB11" s="119"/>
+      <c r="BB11" s="136"/>
       <c r="BC11" s="32" t="str">
         <f>AR15</f>
         <v>Portugal</v>
@@ -33997,10 +33995,10 @@
         <f>AB22</f>
         <v>Peru</v>
       </c>
-      <c r="F12" s="152">
-        <v>0</v>
-      </c>
-      <c r="G12" s="153">
+      <c r="F12" s="111">
+        <v>0</v>
+      </c>
+      <c r="G12" s="112">
         <v>1</v>
       </c>
       <c r="H12" s="93" t="str">
@@ -34134,7 +34132,7 @@
       <c r="BF12" s="27"/>
       <c r="BG12" s="36"/>
       <c r="BH12" s="27"/>
-      <c r="BI12" s="118">
+      <c r="BI12" s="135">
         <v>57</v>
       </c>
       <c r="BJ12" s="30" t="str">
@@ -34179,10 +34177,10 @@
         <f>AB26</f>
         <v>Argentina</v>
       </c>
-      <c r="F13" s="152">
+      <c r="F13" s="111">
         <v>1</v>
       </c>
-      <c r="G13" s="153">
+      <c r="G13" s="112">
         <v>1</v>
       </c>
       <c r="H13" s="93" t="str">
@@ -34248,7 +34246,7 @@
       <c r="BF13" s="35"/>
       <c r="BG13" s="36"/>
       <c r="BH13" s="39"/>
-      <c r="BI13" s="119"/>
+      <c r="BI13" s="136"/>
       <c r="BJ13" s="32" t="str">
         <f>T59</f>
         <v>W50</v>
@@ -34291,10 +34289,10 @@
         <f>AB28</f>
         <v>Croatia</v>
       </c>
-      <c r="F14" s="152">
+      <c r="F14" s="111">
         <v>2</v>
       </c>
-      <c r="G14" s="153">
+      <c r="G14" s="112">
         <v>0</v>
       </c>
       <c r="H14" s="93" t="str">
@@ -34453,7 +34451,7 @@
         <f>AU14-AV14</f>
         <v>0</v>
       </c>
-      <c r="BB14" s="118">
+      <c r="BB14" s="135">
         <v>50</v>
       </c>
       <c r="BC14" s="30" t="str">
@@ -34505,10 +34503,10 @@
         <f>AB32</f>
         <v>Brazil</v>
       </c>
-      <c r="F15" s="152">
+      <c r="F15" s="111">
         <v>1</v>
       </c>
-      <c r="G15" s="153">
+      <c r="G15" s="112">
         <v>1</v>
       </c>
       <c r="H15" s="93" t="str">
@@ -34667,7 +34665,7 @@
         <f>AU15-AV15</f>
         <v>0</v>
       </c>
-      <c r="BB15" s="119"/>
+      <c r="BB15" s="136"/>
       <c r="BC15" s="32" t="str">
         <f>AR27</f>
         <v>Argentina</v>
@@ -34720,10 +34718,10 @@
         <f>AB34</f>
         <v>Costa Rica</v>
       </c>
-      <c r="F16" s="152">
-        <v>0</v>
-      </c>
-      <c r="G16" s="153">
+      <c r="F16" s="111">
+        <v>0</v>
+      </c>
+      <c r="G16" s="112">
         <v>1</v>
       </c>
       <c r="H16" s="93" t="str">
@@ -34892,7 +34890,7 @@
       <c r="BM16" s="27"/>
       <c r="BN16" s="36"/>
       <c r="BO16" s="27"/>
-      <c r="BP16" s="118">
+      <c r="BP16" s="135">
         <v>61</v>
       </c>
       <c r="BQ16" s="30" t="str">
@@ -34930,10 +34928,10 @@
         <f>AB38</f>
         <v>Germany</v>
       </c>
-      <c r="F17" s="152">
-        <v>0</v>
-      </c>
-      <c r="G17" s="153">
+      <c r="F17" s="111">
+        <v>0</v>
+      </c>
+      <c r="G17" s="112">
         <v>1</v>
       </c>
       <c r="H17" s="93" t="str">
@@ -35105,7 +35103,7 @@
       <c r="BM17" s="27"/>
       <c r="BN17" s="36"/>
       <c r="BO17" s="39"/>
-      <c r="BP17" s="119"/>
+      <c r="BP17" s="136"/>
       <c r="BQ17" s="32" t="str">
         <f>T70</f>
         <v>W58</v>
@@ -35141,10 +35139,10 @@
         <f>AB40</f>
         <v>Sweden</v>
       </c>
-      <c r="F18" s="152">
+      <c r="F18" s="111">
         <v>1</v>
       </c>
-      <c r="G18" s="153">
+      <c r="G18" s="112">
         <v>0</v>
       </c>
       <c r="H18" s="93" t="str">
@@ -35271,7 +35269,7 @@
         <f>MAX(AW14:AW17)-MIN(AW14:AW17)+1</f>
         <v>1</v>
       </c>
-      <c r="BB18" s="118">
+      <c r="BB18" s="135">
         <v>53</v>
       </c>
       <c r="BC18" s="30" t="str">
@@ -35323,10 +35321,10 @@
         <f>AB44</f>
         <v>Belgium</v>
       </c>
-      <c r="F19" s="152">
+      <c r="F19" s="111">
         <v>3</v>
       </c>
-      <c r="G19" s="153">
+      <c r="G19" s="112">
         <v>0</v>
       </c>
       <c r="H19" s="93" t="str">
@@ -35382,7 +35380,7 @@
       </c>
       <c r="AO19" s="101"/>
       <c r="AP19" s="101"/>
-      <c r="BB19" s="119"/>
+      <c r="BB19" s="136"/>
       <c r="BC19" s="32" t="str">
         <f>AR39</f>
         <v>Mexico</v>
@@ -35435,10 +35433,10 @@
         <f>AB46</f>
         <v>Tunisia</v>
       </c>
-      <c r="F20" s="152">
+      <c r="F20" s="111">
         <v>1</v>
       </c>
-      <c r="G20" s="153">
+      <c r="G20" s="112">
         <v>2</v>
       </c>
       <c r="H20" s="93" t="str">
@@ -35604,7 +35602,7 @@
       <c r="BF20" s="27"/>
       <c r="BG20" s="36"/>
       <c r="BH20" s="27"/>
-      <c r="BI20" s="118">
+      <c r="BI20" s="135">
         <v>58</v>
       </c>
       <c r="BJ20" s="30" t="str">
@@ -35649,10 +35647,10 @@
         <f>AB50</f>
         <v>Poland</v>
       </c>
-      <c r="F21" s="152">
+      <c r="F21" s="111">
         <v>1</v>
       </c>
-      <c r="G21" s="153">
+      <c r="G21" s="112">
         <v>2</v>
       </c>
       <c r="H21" s="93" t="str">
@@ -35821,7 +35819,7 @@
       <c r="BF21" s="35"/>
       <c r="BG21" s="36"/>
       <c r="BH21" s="39"/>
-      <c r="BI21" s="119"/>
+      <c r="BI21" s="136"/>
       <c r="BJ21" s="32" t="str">
         <f>T63</f>
         <v>W54</v>
@@ -35864,10 +35862,10 @@
         <f>AB52</f>
         <v>Colombia</v>
       </c>
-      <c r="F22" s="152">
+      <c r="F22" s="111">
         <v>1</v>
       </c>
-      <c r="G22" s="153">
+      <c r="G22" s="112">
         <v>2</v>
       </c>
       <c r="H22" s="93" t="str">
@@ -36022,12 +36020,12 @@
         <f>AU22-AV22</f>
         <v>0</v>
       </c>
-      <c r="BB22" s="118">
+      <c r="BB22" s="135">
         <v>54</v>
       </c>
       <c r="BC22" s="30" t="str">
         <f>AR44</f>
-        <v>1G</v>
+        <v>Belgium</v>
       </c>
       <c r="BD22" s="88"/>
       <c r="BE22" s="90"/>
@@ -36077,10 +36075,10 @@
         <f>AB8</f>
         <v>Russia</v>
       </c>
-      <c r="F23" s="152">
+      <c r="F23" s="111">
         <v>3</v>
       </c>
-      <c r="G23" s="153">
+      <c r="G23" s="112">
         <v>1</v>
       </c>
       <c r="H23" s="93" t="str">
@@ -36235,7 +36233,7 @@
         <f>AU23-AV23</f>
         <v>0</v>
       </c>
-      <c r="BB23" s="119"/>
+      <c r="BB23" s="136"/>
       <c r="BC23" s="32" t="str">
         <f>AR51</f>
         <v>Japan</v>
@@ -36259,7 +36257,7 @@
       <c r="BT23" s="27"/>
       <c r="BU23" s="36"/>
       <c r="BV23" s="27"/>
-      <c r="BW23" s="118">
+      <c r="BW23" s="135">
         <v>64</v>
       </c>
       <c r="BX23" s="30" t="str">
@@ -36290,10 +36288,10 @@
         <f>AB11</f>
         <v>Uruguay</v>
       </c>
-      <c r="F24" s="152">
+      <c r="F24" s="111">
         <v>1</v>
       </c>
-      <c r="G24" s="153">
+      <c r="G24" s="112">
         <v>0</v>
       </c>
       <c r="H24" s="93" t="str">
@@ -36440,7 +36438,7 @@
       <c r="BT24" s="27"/>
       <c r="BU24" s="36"/>
       <c r="BV24" s="39"/>
-      <c r="BW24" s="119"/>
+      <c r="BW24" s="136"/>
       <c r="BX24" s="32" t="str">
         <f>T77</f>
         <v>W62</v>
@@ -36469,10 +36467,10 @@
         <f>AB14</f>
         <v>Portugal</v>
       </c>
-      <c r="F25" s="152">
+      <c r="F25" s="111">
         <v>1</v>
       </c>
-      <c r="G25" s="153">
+      <c r="G25" s="112">
         <v>0</v>
       </c>
       <c r="H25" s="93" t="str">
@@ -36578,10 +36576,10 @@
         <f>AB17</f>
         <v>Iran</v>
       </c>
-      <c r="F26" s="152">
-        <v>0</v>
-      </c>
-      <c r="G26" s="153">
+      <c r="F26" s="111">
+        <v>0</v>
+      </c>
+      <c r="G26" s="112">
         <v>1</v>
       </c>
       <c r="H26" s="93" t="str">
@@ -36740,7 +36738,7 @@
         <f>AU26-AV26</f>
         <v>0</v>
       </c>
-      <c r="BB26" s="118">
+      <c r="BB26" s="135">
         <v>51</v>
       </c>
       <c r="BC26" s="30" t="str">
@@ -36792,10 +36790,10 @@
         <f>AB20</f>
         <v>France</v>
       </c>
-      <c r="F27" s="152">
+      <c r="F27" s="111">
         <v>1</v>
       </c>
-      <c r="G27" s="153">
+      <c r="G27" s="112">
         <v>0</v>
       </c>
       <c r="H27" s="93" t="str">
@@ -36954,7 +36952,7 @@
         <f>AU27-AV27</f>
         <v>0</v>
       </c>
-      <c r="BB27" s="119"/>
+      <c r="BB27" s="136"/>
       <c r="BC27" s="32" t="str">
         <f>AR9</f>
         <v>Russia</v>
@@ -37007,10 +37005,10 @@
         <f>AB23</f>
         <v>Denmark</v>
       </c>
-      <c r="F28" s="152">
+      <c r="F28" s="111">
         <v>1</v>
       </c>
-      <c r="G28" s="153">
+      <c r="G28" s="112">
         <v>1</v>
       </c>
       <c r="H28" s="93" t="str">
@@ -37172,7 +37170,7 @@
       <c r="BF28" s="27"/>
       <c r="BG28" s="36"/>
       <c r="BH28" s="27"/>
-      <c r="BI28" s="118">
+      <c r="BI28" s="135">
         <v>59</v>
       </c>
       <c r="BJ28" s="30" t="str">
@@ -37217,10 +37215,10 @@
         <f>AB26</f>
         <v>Argentina</v>
       </c>
-      <c r="F29" s="152">
-        <v>0</v>
-      </c>
-      <c r="G29" s="153">
+      <c r="F29" s="111">
+        <v>0</v>
+      </c>
+      <c r="G29" s="112">
         <v>3</v>
       </c>
       <c r="H29" s="93" t="str">
@@ -37337,11 +37335,11 @@
       </c>
       <c r="AM29" s="101">
         <f>VLOOKUP(AB29,fair_play,2,FALSE)</f>
-        <v>-8</v>
+        <v>-11</v>
       </c>
       <c r="AN29" s="101">
         <f t="shared" si="19"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AO29" s="101">
         <f>VLOOKUP(AB29,fair_play,3,FALSE)</f>
@@ -37353,7 +37351,7 @@
       </c>
       <c r="AQ29" s="102">
         <f>1000*AK29/AK30+100*AJ29+10*AF29/AF30+1*AL29/AL30+0.00001*AN29+0.000001*AP29</f>
-        <v>358.33335433333332</v>
+        <v>358.33334433333329</v>
       </c>
       <c r="AS29" s="104">
         <f>SUMPRODUCT(($S$7:$S$54=AB29&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB29&amp;"_win")*($U$7:$U$54))</f>
@@ -37385,7 +37383,7 @@
       <c r="BF29" s="35"/>
       <c r="BG29" s="36"/>
       <c r="BH29" s="39"/>
-      <c r="BI29" s="119"/>
+      <c r="BI29" s="136"/>
       <c r="BJ29" s="32" t="str">
         <f>T61</f>
         <v>W52</v>
@@ -37428,10 +37426,10 @@
         <f>AB29</f>
         <v>Nigeria</v>
       </c>
-      <c r="F30" s="152">
+      <c r="F30" s="111">
         <v>2</v>
       </c>
-      <c r="G30" s="153">
+      <c r="G30" s="112">
         <v>0</v>
       </c>
       <c r="H30" s="93" t="str">
@@ -37558,7 +37556,7 @@
         <f>MAX(AW26:AW29)-MIN(AW26:AW29)+1</f>
         <v>1</v>
       </c>
-      <c r="BB30" s="118">
+      <c r="BB30" s="135">
         <v>52</v>
       </c>
       <c r="BC30" s="30" t="str">
@@ -37610,10 +37608,10 @@
         <f>AB32</f>
         <v>Brazil</v>
       </c>
-      <c r="F31" s="152">
+      <c r="F31" s="111">
         <v>2</v>
       </c>
-      <c r="G31" s="153">
+      <c r="G31" s="112">
         <v>0</v>
       </c>
       <c r="H31" s="93" t="str">
@@ -37662,7 +37660,7 @@
       </c>
       <c r="AO31" s="101"/>
       <c r="AP31" s="101"/>
-      <c r="BB31" s="119"/>
+      <c r="BB31" s="136"/>
       <c r="BC31" s="32" t="str">
         <f>AR21</f>
         <v>Denmark</v>
@@ -37689,14 +37687,14 @@
       <c r="BT31" s="35"/>
       <c r="BU31" s="36"/>
       <c r="BV31" s="41"/>
-      <c r="BW31" s="124" t="str">
+      <c r="BW31" s="137" t="str">
         <f>INDEX(T,7,lang)</f>
         <v>Third-Place Play-Off</v>
       </c>
-      <c r="BX31" s="125"/>
-      <c r="BY31" s="125"/>
-      <c r="BZ31" s="125"/>
-      <c r="CA31" s="126"/>
+      <c r="BX31" s="138"/>
+      <c r="BY31" s="138"/>
+      <c r="BZ31" s="138"/>
+      <c r="CA31" s="139"/>
     </row>
     <row r="32" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="23">
@@ -37718,10 +37716,10 @@
         <f>AB35</f>
         <v>Serbia</v>
       </c>
-      <c r="F32" s="152">
+      <c r="F32" s="111">
         <v>1</v>
       </c>
-      <c r="G32" s="153">
+      <c r="G32" s="112">
         <v>2</v>
       </c>
       <c r="H32" s="93" t="str">
@@ -37894,7 +37892,7 @@
       <c r="BM32" s="27"/>
       <c r="BN32" s="36"/>
       <c r="BO32" s="27"/>
-      <c r="BP32" s="118">
+      <c r="BP32" s="135">
         <v>62</v>
       </c>
       <c r="BQ32" s="30" t="str">
@@ -37906,11 +37904,11 @@
       <c r="BT32" s="31"/>
       <c r="BU32" s="40"/>
       <c r="BV32" s="41"/>
-      <c r="BW32" s="127"/>
-      <c r="BX32" s="128"/>
-      <c r="BY32" s="128"/>
-      <c r="BZ32" s="128"/>
-      <c r="CA32" s="129"/>
+      <c r="BW32" s="140"/>
+      <c r="BX32" s="141"/>
+      <c r="BY32" s="141"/>
+      <c r="BZ32" s="141"/>
+      <c r="CA32" s="142"/>
     </row>
     <row r="33" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="23">
@@ -37932,10 +37930,10 @@
         <f>AB38</f>
         <v>Germany</v>
       </c>
-      <c r="F33" s="152">
+      <c r="F33" s="111">
         <v>2</v>
       </c>
-      <c r="G33" s="153">
+      <c r="G33" s="112">
         <v>1</v>
       </c>
       <c r="H33" s="93" t="str">
@@ -38111,7 +38109,7 @@
       <c r="BM33" s="27"/>
       <c r="BN33" s="36"/>
       <c r="BO33" s="39"/>
-      <c r="BP33" s="119"/>
+      <c r="BP33" s="136"/>
       <c r="BQ33" s="32" t="str">
         <f>T72</f>
         <v>W60</v>
@@ -38147,10 +38145,10 @@
         <f>AB41</f>
         <v>Korea Republic</v>
       </c>
-      <c r="F34" s="152">
+      <c r="F34" s="111">
         <v>1</v>
       </c>
-      <c r="G34" s="153">
+      <c r="G34" s="112">
         <v>2</v>
       </c>
       <c r="H34" s="93" t="str">
@@ -38305,7 +38303,7 @@
         <f>AU34-AV34</f>
         <v>0</v>
       </c>
-      <c r="BB34" s="118">
+      <c r="BB34" s="135">
         <v>55</v>
       </c>
       <c r="BC34" s="30" t="str">
@@ -38360,10 +38358,10 @@
         <f>AB44</f>
         <v>Belgium</v>
       </c>
-      <c r="F35" s="152">
+      <c r="F35" s="111">
         <v>5</v>
       </c>
-      <c r="G35" s="153">
+      <c r="G35" s="112">
         <v>2</v>
       </c>
       <c r="H35" s="93" t="str">
@@ -38518,7 +38516,7 @@
         <f>AU35-AV35</f>
         <v>0</v>
       </c>
-      <c r="BB35" s="119"/>
+      <c r="BB35" s="136"/>
       <c r="BC35" s="32" t="str">
         <f>AR33</f>
         <v>Switzerland</v>
@@ -38545,7 +38543,7 @@
       <c r="BT35" s="27"/>
       <c r="BU35" s="27"/>
       <c r="BV35" s="27"/>
-      <c r="BW35" s="118">
+      <c r="BW35" s="135">
         <v>63</v>
       </c>
       <c r="BX35" s="30" t="str">
@@ -38576,10 +38574,10 @@
         <f>AB47</f>
         <v>England</v>
       </c>
-      <c r="F36" s="152">
+      <c r="F36" s="111">
         <v>6</v>
       </c>
-      <c r="G36" s="153">
+      <c r="G36" s="112">
         <v>1</v>
       </c>
       <c r="H36" s="93" t="str">
@@ -38713,7 +38711,7 @@
       <c r="BF36" s="27"/>
       <c r="BG36" s="36"/>
       <c r="BH36" s="27"/>
-      <c r="BI36" s="118">
+      <c r="BI36" s="135">
         <v>60</v>
       </c>
       <c r="BJ36" s="30" t="str">
@@ -38732,7 +38730,7 @@
       <c r="BT36" s="27"/>
       <c r="BU36" s="27"/>
       <c r="BV36" s="27"/>
-      <c r="BW36" s="119"/>
+      <c r="BW36" s="136"/>
       <c r="BX36" s="32" t="str">
         <f>Z77</f>
         <v>L62</v>
@@ -38761,10 +38759,10 @@
         <f>AB50</f>
         <v>Poland</v>
       </c>
-      <c r="F37" s="152">
-        <v>0</v>
-      </c>
-      <c r="G37" s="153">
+      <c r="F37" s="111">
+        <v>0</v>
+      </c>
+      <c r="G37" s="112">
         <v>3</v>
       </c>
       <c r="H37" s="93" t="str">
@@ -38823,7 +38821,7 @@
       <c r="BF37" s="35"/>
       <c r="BG37" s="36"/>
       <c r="BH37" s="39"/>
-      <c r="BI37" s="119"/>
+      <c r="BI37" s="136"/>
       <c r="BJ37" s="32" t="str">
         <f>T65</f>
         <v>W56</v>
@@ -38866,10 +38864,10 @@
         <f>AB53</f>
         <v>Japan</v>
       </c>
-      <c r="F38" s="152">
+      <c r="F38" s="111">
         <v>2</v>
       </c>
-      <c r="G38" s="153">
+      <c r="G38" s="112">
         <v>2</v>
       </c>
       <c r="H38" s="93" t="str">
@@ -39028,7 +39026,7 @@
         <f>AU38-AV38</f>
         <v>0</v>
       </c>
-      <c r="BB38" s="118">
+      <c r="BB38" s="135">
         <v>56</v>
       </c>
       <c r="BC38" s="30" t="str">
@@ -39075,10 +39073,10 @@
         <f>AB11</f>
         <v>Uruguay</v>
       </c>
-      <c r="F39" s="152">
+      <c r="F39" s="111">
         <v>3</v>
       </c>
-      <c r="G39" s="153">
+      <c r="G39" s="112">
         <v>0</v>
       </c>
       <c r="H39" s="93" t="str">
@@ -39237,10 +39235,10 @@
         <f>AU39-AV39</f>
         <v>0</v>
       </c>
-      <c r="BB39" s="119"/>
+      <c r="BB39" s="136"/>
       <c r="BC39" s="32" t="str">
         <f>AR45</f>
-        <v>2G</v>
+        <v>England</v>
       </c>
       <c r="BD39" s="89"/>
       <c r="BE39" s="91"/>
@@ -39280,10 +39278,10 @@
         <f>AB9</f>
         <v>Saudi Arabia</v>
       </c>
-      <c r="F40" s="152">
+      <c r="F40" s="111">
         <v>2</v>
       </c>
-      <c r="G40" s="153">
+      <c r="G40" s="112">
         <v>1</v>
       </c>
       <c r="H40" s="93" t="str">
@@ -39459,10 +39457,10 @@
         <f>AB17</f>
         <v>Iran</v>
       </c>
-      <c r="F41" s="152">
+      <c r="F41" s="111">
         <v>1</v>
       </c>
-      <c r="G41" s="153">
+      <c r="G41" s="112">
         <v>1</v>
       </c>
       <c r="H41" s="93" t="str">
@@ -39617,25 +39615,25 @@
         <f>AU41-AV41</f>
         <v>0</v>
       </c>
-      <c r="BO41" s="120" t="str">
+      <c r="BO41" s="152" t="str">
         <f>INDEX(T,102,lang)</f>
         <v>World Champion 2018</v>
       </c>
-      <c r="BP41" s="120"/>
-      <c r="BQ41" s="120"/>
-      <c r="BR41" s="120"/>
-      <c r="BS41" s="120"/>
-      <c r="BT41" s="120"/>
-      <c r="BU41" s="122" t="str">
+      <c r="BP41" s="152"/>
+      <c r="BQ41" s="152"/>
+      <c r="BR41" s="152"/>
+      <c r="BS41" s="152"/>
+      <c r="BT41" s="152"/>
+      <c r="BU41" s="154" t="str">
         <f>S85</f>
         <v/>
       </c>
-      <c r="BV41" s="122"/>
-      <c r="BW41" s="122"/>
-      <c r="BX41" s="122"/>
-      <c r="BY41" s="122"/>
-      <c r="BZ41" s="122"/>
-      <c r="CA41" s="122"/>
+      <c r="BV41" s="154"/>
+      <c r="BW41" s="154"/>
+      <c r="BX41" s="154"/>
+      <c r="BY41" s="154"/>
+      <c r="BZ41" s="154"/>
+      <c r="CA41" s="154"/>
     </row>
     <row r="42" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="23">
@@ -39657,10 +39655,10 @@
         <f>AB15</f>
         <v>Spain</v>
       </c>
-      <c r="F42" s="152">
+      <c r="F42" s="111">
         <v>2</v>
       </c>
-      <c r="G42" s="153">
+      <c r="G42" s="112">
         <v>2</v>
       </c>
       <c r="H42" s="93" t="str">
@@ -39787,19 +39785,19 @@
         <f>MAX(AW38:AW41)-MIN(AW38:AW41)+1</f>
         <v>1</v>
       </c>
-      <c r="BO42" s="121"/>
-      <c r="BP42" s="121"/>
-      <c r="BQ42" s="121"/>
-      <c r="BR42" s="121"/>
-      <c r="BS42" s="121"/>
-      <c r="BT42" s="121"/>
-      <c r="BU42" s="123"/>
-      <c r="BV42" s="123"/>
-      <c r="BW42" s="123"/>
-      <c r="BX42" s="123"/>
-      <c r="BY42" s="123"/>
-      <c r="BZ42" s="123"/>
-      <c r="CA42" s="123"/>
+      <c r="BO42" s="153"/>
+      <c r="BP42" s="153"/>
+      <c r="BQ42" s="153"/>
+      <c r="BR42" s="153"/>
+      <c r="BS42" s="153"/>
+      <c r="BT42" s="153"/>
+      <c r="BU42" s="155"/>
+      <c r="BV42" s="155"/>
+      <c r="BW42" s="155"/>
+      <c r="BX42" s="155"/>
+      <c r="BY42" s="155"/>
+      <c r="BZ42" s="155"/>
+      <c r="CA42" s="155"/>
     </row>
     <row r="43" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="23">
@@ -39821,10 +39819,10 @@
         <f>AB23</f>
         <v>Denmark</v>
       </c>
-      <c r="F43" s="152">
-        <v>0</v>
-      </c>
-      <c r="G43" s="153">
+      <c r="F43" s="111">
+        <v>0</v>
+      </c>
+      <c r="G43" s="112">
         <v>0</v>
       </c>
       <c r="H43" s="93" t="str">
@@ -39895,10 +39893,10 @@
         <f>AB21</f>
         <v>Australia</v>
       </c>
-      <c r="F44" s="152">
-        <v>0</v>
-      </c>
-      <c r="G44" s="153">
+      <c r="F44" s="111">
+        <v>0</v>
+      </c>
+      <c r="G44" s="112">
         <v>2</v>
       </c>
       <c r="H44" s="93" t="str">
@@ -39967,7 +39965,7 @@
       </c>
       <c r="AA44" s="101">
         <f>COUNTIF(AQ44:AQ47,CONCATENATE("&gt;=",AQ44))</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AB44" s="102" t="str">
         <f>VLOOKUP("Belgium",T,lang,FALSE)</f>
@@ -39975,7 +39973,7 @@
       </c>
       <c r="AC44" s="101">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB44 &amp; "_win")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AD44" s="101">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB44 &amp; "_draw")</f>
@@ -39987,7 +39985,7 @@
       </c>
       <c r="AF44" s="101">
         <f>SUMIF($E$7:$E$54,$AB44,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB44,$G$7:$G$54)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="AG44" s="101">
         <f>SUMIF($E$7:$E$54,$AB44,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB44,$F$7:$F$54)</f>
@@ -39995,19 +39993,19 @@
       </c>
       <c r="AH44" s="101">
         <f>(AF44-AG44)*100+AK44*10000+AF44</f>
-        <v>60608</v>
+        <v>90709</v>
       </c>
       <c r="AI44" s="101">
         <f>AF44-AG44</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AJ44" s="101">
         <f>(AI44-AI49)/AI48</f>
-        <v>0.93333333333333335</v>
+        <v>0.94117647058823528</v>
       </c>
       <c r="AK44" s="101">
         <f>AC44*3+AD44</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AL44" s="101">
         <f>AS44/AS48*1000+AT44/AT48*100+AW44/AW48*10+AU44/AU48</f>
@@ -40015,7 +40013,7 @@
       </c>
       <c r="AM44" s="101">
         <f>VLOOKUP(AB44,fair_play,2,FALSE)</f>
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="AN44" s="101">
         <f>COUNTIF($AM$44:$AM$47,CONCATENATE("&lt;=",AM44))</f>
@@ -40031,11 +40029,11 @@
       </c>
       <c r="AQ44" s="102">
         <f>1000*AK44/AK48+100*AJ44+10*AF44/AF48+1*AL44/AL48+0.00001*AN44+0.000001*AP44</f>
-        <v>960.47621447619042</v>
+        <v>1005.3676710588235</v>
       </c>
       <c r="AR44" s="103" t="str">
         <f>IF(SUM(AC44:AE47)=12,J45,INDEX(T,82,lang))</f>
-        <v>1G</v>
+        <v>Belgium</v>
       </c>
       <c r="AS44" s="104">
         <f>SUMPRODUCT(($S$7:$S$54=AB44&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB44&amp;"_win")*($U$7:$U$54))</f>
@@ -40078,10 +40076,10 @@
         <f>AB29</f>
         <v>Nigeria</v>
       </c>
-      <c r="F45" s="152">
+      <c r="F45" s="111">
         <v>1</v>
       </c>
-      <c r="G45" s="153">
+      <c r="G45" s="112">
         <v>2</v>
       </c>
       <c r="H45" s="93" t="str">
@@ -40090,15 +40088,15 @@
       </c>
       <c r="J45" s="58" t="str">
         <f>VLOOKUP(1,AA44:AK47,2,FALSE)</f>
-        <v>England</v>
+        <v>Belgium</v>
       </c>
       <c r="K45" s="59">
         <f>L45+M45+N45</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L45" s="59">
         <f>VLOOKUP(1,AA44:AK47,3,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M45" s="59">
         <f>VLOOKUP(1,AA44:AK47,4,FALSE)</f>
@@ -40110,11 +40108,11 @@
       </c>
       <c r="O45" s="59" t="str">
         <f>VLOOKUP(1,AA44:AK47,6,FALSE) &amp; " - " &amp; VLOOKUP(1,AA44:AK47,7,FALSE)</f>
-        <v>8 - 2</v>
+        <v>9 - 2</v>
       </c>
       <c r="P45" s="60">
         <f>L45*3+M45</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="R45" s="101">
         <f>DATE(2018,6,26)+TIME(7,0,0)+gmt_delta</f>
@@ -40166,23 +40164,23 @@
       </c>
       <c r="AE45" s="101">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB45 &amp; "_lose")</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AF45" s="101">
         <f>SUMIF($E$7:$E$54,$AB45,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB45,$G$7:$G$54)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AG45" s="101">
         <f>SUMIF($E$7:$E$54,$AB45,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB45,$F$7:$F$54)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="AH45" s="101">
         <f>(AF45-AG45)*100+AK45*10000+AF45</f>
-        <v>-799</v>
+        <v>-898</v>
       </c>
       <c r="AI45" s="101">
         <f>AF45-AG45</f>
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="AJ45" s="101">
         <f>(AI45-AI49)/AI48</f>
@@ -40202,7 +40200,7 @@
       </c>
       <c r="AN45" s="101">
         <f t="shared" ref="AN45:AN47" si="28">COUNTIF($AM$44:$AM$47,CONCATENATE("&lt;=",AM45))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AO45" s="101">
         <f>VLOOKUP(AB45,fair_play,3,FALSE)</f>
@@ -40214,11 +40212,11 @@
       </c>
       <c r="AQ45" s="102">
         <f>1000*AK45/AK48+100*AJ45+10*AF45/AF48+1*AL45/AL48+0.00001*AN45+0.000001*AP45</f>
-        <v>1.2500120000000001</v>
+        <v>2.500022</v>
       </c>
       <c r="AR45" s="103" t="str">
         <f>IF(SUM(AC44:AE47)=12,J46,INDEX(T,83,lang))</f>
-        <v>2G</v>
+        <v>England</v>
       </c>
       <c r="AS45" s="104">
         <f>SUMPRODUCT(($S$7:$S$54=AB45&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB45&amp;"_win")*($U$7:$U$54))</f>
@@ -40261,10 +40259,10 @@
         <f>AB27</f>
         <v>Iceland</v>
       </c>
-      <c r="F46" s="152">
+      <c r="F46" s="111">
         <v>1</v>
       </c>
-      <c r="G46" s="153">
+      <c r="G46" s="112">
         <v>2</v>
       </c>
       <c r="H46" s="93" t="str">
@@ -40273,11 +40271,11 @@
       </c>
       <c r="J46" s="61" t="str">
         <f>VLOOKUP(2,AA44:AK47,2,FALSE)</f>
-        <v>Belgium</v>
+        <v>England</v>
       </c>
       <c r="K46" s="29">
         <f>L46+M46+N46</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L46" s="29">
         <f>VLOOKUP(2,AA44:AK47,3,FALSE)</f>
@@ -40289,11 +40287,11 @@
       </c>
       <c r="N46" s="29">
         <f>VLOOKUP(2,AA44:AK47,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O46" s="29" t="str">
         <f>VLOOKUP(2,AA44:AK47,6,FALSE) &amp; " - " &amp; VLOOKUP(2,AA44:AK47,7,FALSE)</f>
-        <v>8 - 2</v>
+        <v>8 - 3</v>
       </c>
       <c r="P46" s="62">
         <f>L46*3+M46</f>
@@ -40341,7 +40339,7 @@
       </c>
       <c r="AC46" s="101">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB46 &amp; "_win")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AD46" s="101">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB46 &amp; "_draw")</f>
@@ -40353,27 +40351,27 @@
       </c>
       <c r="AF46" s="101">
         <f>SUMIF($E$7:$E$54,$AB46,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB46,$G$7:$G$54)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AG46" s="101">
         <f>SUMIF($E$7:$E$54,$AB46,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB46,$F$7:$F$54)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AH46" s="101">
         <f>(AF46-AG46)*100+AK46*10000+AF46</f>
-        <v>-397</v>
+        <v>29705</v>
       </c>
       <c r="AI46" s="101">
         <f>AF46-AG46</f>
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="AJ46" s="101">
         <f>(AI46-AI49)/AI48</f>
-        <v>0.26666666666666666</v>
+        <v>0.35294117647058826</v>
       </c>
       <c r="AK46" s="101">
         <f>AC46*3+AD46</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AL46" s="101">
         <f>AS46/AS48*1000+AT46/AT48*100+AW46/AW48*10+AU46/AU48</f>
@@ -40381,11 +40379,11 @@
       </c>
       <c r="AM46" s="101">
         <f>VLOOKUP(AB46,fair_play,2,FALSE)</f>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="AN46" s="101">
         <f t="shared" si="28"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AO46" s="101">
         <f>VLOOKUP(AB46,fair_play,3,FALSE)</f>
@@ -40397,7 +40395,7 @@
       </c>
       <c r="AQ46" s="102">
         <f>1000*AK46/AK48+100*AJ46+10*AF46/AF48+1*AL46/AL48+0.00001*AN46+0.000001*AP46</f>
-        <v>30.416707666666667</v>
+        <v>341.54414864705882</v>
       </c>
       <c r="AS46" s="104">
         <f>SUMPRODUCT(($S$7:$S$54=AB46&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB46&amp;"_win")*($U$7:$U$54))</f>
@@ -40419,13 +40417,13 @@
         <f>AU46-AV46</f>
         <v>0</v>
       </c>
-      <c r="BB46" s="109" t="s">
+      <c r="BB46" s="143" t="s">
         <v>2219</v>
       </c>
-      <c r="BC46" s="110"/>
-      <c r="BD46" s="110"/>
-      <c r="BE46" s="110"/>
-      <c r="BF46" s="111"/>
+      <c r="BC46" s="144"/>
+      <c r="BD46" s="144"/>
+      <c r="BE46" s="144"/>
+      <c r="BF46" s="145"/>
     </row>
     <row r="47" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="23">
@@ -40447,10 +40445,10 @@
         <f>AB35</f>
         <v>Serbia</v>
       </c>
-      <c r="F47" s="152">
-        <v>0</v>
-      </c>
-      <c r="G47" s="153">
+      <c r="F47" s="111">
+        <v>0</v>
+      </c>
+      <c r="G47" s="112">
         <v>2</v>
       </c>
       <c r="H47" s="93" t="str">
@@ -40463,11 +40461,11 @@
       </c>
       <c r="K47" s="29">
         <f>L47+M47+N47</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L47" s="29">
         <f>VLOOKUP(3,AA44:AK47,3,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M47" s="29">
         <f>VLOOKUP(3,AA44:AK47,4,FALSE)</f>
@@ -40479,11 +40477,11 @@
       </c>
       <c r="O47" s="29" t="str">
         <f>VLOOKUP(3,AA44:AK47,6,FALSE) &amp; " - " &amp; VLOOKUP(3,AA44:AK47,7,FALSE)</f>
-        <v>3 - 7</v>
+        <v>5 - 8</v>
       </c>
       <c r="P47" s="62">
         <f>L47*3+M47</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R47" s="101">
         <f>DATE(2018,6,27)+TIME(7,0,0)+gmt_delta</f>
@@ -40519,7 +40517,7 @@
       </c>
       <c r="AA47" s="101">
         <f>COUNTIF(AQ44:AQ47,CONCATENATE("&gt;=",AQ47))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB47" s="102" t="str">
         <f>VLOOKUP("England",T,lang,FALSE)</f>
@@ -40535,7 +40533,7 @@
       </c>
       <c r="AE47" s="101">
         <f>COUNTIF($S$7:$T$54,"=" &amp; AB47 &amp; "_lose")</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AF47" s="101">
         <f>SUMIF($E$7:$E$54,$AB47,$F$7:$F$54) + SUMIF($H$7:$H$54,$AB47,$G$7:$G$54)</f>
@@ -40543,19 +40541,19 @@
       </c>
       <c r="AG47" s="101">
         <f>SUMIF($E$7:$E$54,$AB47,$G$7:$G$54) + SUMIF($H$7:$H$54,$AB47,$F$7:$F$54)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AH47" s="101">
         <f>(AF47-AG47)*100+AK47*10000+AF47</f>
-        <v>60608</v>
+        <v>60508</v>
       </c>
       <c r="AI47" s="101">
         <f>AF47-AG47</f>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="AJ47" s="101">
         <f>(AI47-AI49)/AI48</f>
-        <v>0.93333333333333335</v>
+        <v>0.82352941176470584</v>
       </c>
       <c r="AK47" s="101">
         <f>AC47*3+AD47</f>
@@ -40571,7 +40569,7 @@
       </c>
       <c r="AN47" s="101">
         <f t="shared" si="28"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AO47" s="101">
         <f>VLOOKUP(AB47,fair_play,3,FALSE)</f>
@@ -40583,7 +40581,7 @@
       </c>
       <c r="AQ47" s="102">
         <f>1000*AK47/AK48+100*AJ47+10*AF47/AF48+1*AL47/AL48+0.00001*AN47+0.000001*AP47</f>
-        <v>960.47622347619051</v>
+        <v>692.35298417647061</v>
       </c>
       <c r="AS47" s="104">
         <f>SUMPRODUCT(($S$7:$S$54=AB47&amp;"_win")*($U$7:$U$54))+SUMPRODUCT(($T$7:$T$54=AB47&amp;"_win")*($U$7:$U$54))</f>
@@ -40605,11 +40603,11 @@
         <f>AU47-AV47</f>
         <v>0</v>
       </c>
-      <c r="BB47" s="112"/>
-      <c r="BC47" s="113"/>
-      <c r="BD47" s="113"/>
-      <c r="BE47" s="113"/>
-      <c r="BF47" s="114"/>
+      <c r="BB47" s="146"/>
+      <c r="BC47" s="147"/>
+      <c r="BD47" s="147"/>
+      <c r="BE47" s="147"/>
+      <c r="BF47" s="148"/>
     </row>
     <row r="48" spans="1:79" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="23">
@@ -40631,10 +40629,10 @@
         <f>AB33</f>
         <v>Switzerland</v>
       </c>
-      <c r="F48" s="152">
+      <c r="F48" s="111">
         <v>2</v>
       </c>
-      <c r="G48" s="153">
+      <c r="G48" s="112">
         <v>2</v>
       </c>
       <c r="H48" s="93" t="str">
@@ -40647,7 +40645,7 @@
       </c>
       <c r="K48" s="64">
         <f>L48+M48+N48</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L48" s="64">
         <f>VLOOKUP(4,AA44:AK47,3,FALSE)</f>
@@ -40659,11 +40657,11 @@
       </c>
       <c r="N48" s="64">
         <f>VLOOKUP(4,AA44:AK47,5,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="O48" s="64" t="str">
         <f>VLOOKUP(4,AA44:AK47,6,FALSE) &amp; " - " &amp; VLOOKUP(4,AA44:AK47,7,FALSE)</f>
-        <v>1 - 9</v>
+        <v>2 - 11</v>
       </c>
       <c r="P48" s="65">
         <f>L48*3+M48</f>
@@ -40703,7 +40701,7 @@
       </c>
       <c r="AC48" s="101">
         <f t="shared" ref="AC48:AL48" si="30">MAX(AC44:AC47)-MIN(AC44:AC47)+1</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AD48" s="101">
         <f t="shared" si="30"/>
@@ -40711,7 +40709,7 @@
       </c>
       <c r="AE48" s="101">
         <f t="shared" si="30"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AF48" s="101">
         <f t="shared" si="30"/>
@@ -40719,19 +40717,19 @@
       </c>
       <c r="AG48" s="101">
         <f t="shared" si="30"/>
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="AH48" s="101">
         <f>MAX(AH44:AH47)-AH49+1</f>
-        <v>61408</v>
+        <v>91608</v>
       </c>
       <c r="AI48" s="101">
         <f>MAX(AI44:AI47)-AI49+1</f>
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="AK48" s="101">
         <f t="shared" si="30"/>
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="AL48" s="101">
         <f t="shared" si="30"/>
@@ -40761,11 +40759,11 @@
         <f>MAX(AW44:AW47)-MIN(AW44:AW47)+1</f>
         <v>1</v>
       </c>
-      <c r="BB48" s="112"/>
-      <c r="BC48" s="113"/>
-      <c r="BD48" s="113"/>
-      <c r="BE48" s="113"/>
-      <c r="BF48" s="114"/>
+      <c r="BB48" s="146"/>
+      <c r="BC48" s="147"/>
+      <c r="BD48" s="147"/>
+      <c r="BE48" s="147"/>
+      <c r="BF48" s="148"/>
     </row>
     <row r="49" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="23">
@@ -40787,10 +40785,10 @@
         <f>AB41</f>
         <v>Korea Republic</v>
       </c>
-      <c r="F49" s="152">
+      <c r="F49" s="111">
         <v>2</v>
       </c>
-      <c r="G49" s="153">
+      <c r="G49" s="112">
         <v>0</v>
       </c>
       <c r="H49" s="93" t="str">
@@ -40831,19 +40829,19 @@
       </c>
       <c r="AH49" s="101">
         <f>MIN(AH44:AH47)</f>
-        <v>-799</v>
+        <v>-898</v>
       </c>
       <c r="AI49" s="101">
         <f>MIN(AI44:AI47)</f>
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="AO49" s="101"/>
       <c r="AP49" s="101"/>
-      <c r="BB49" s="112"/>
-      <c r="BC49" s="113"/>
-      <c r="BD49" s="113"/>
-      <c r="BE49" s="113"/>
-      <c r="BF49" s="114"/>
+      <c r="BB49" s="146"/>
+      <c r="BC49" s="147"/>
+      <c r="BD49" s="147"/>
+      <c r="BE49" s="147"/>
+      <c r="BF49" s="148"/>
     </row>
     <row r="50" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="23">
@@ -40865,10 +40863,10 @@
         <f>AB39</f>
         <v>Mexico</v>
       </c>
-      <c r="F50" s="152">
-        <v>0</v>
-      </c>
-      <c r="G50" s="153">
+      <c r="F50" s="111">
+        <v>0</v>
+      </c>
+      <c r="G50" s="112">
         <v>3</v>
       </c>
       <c r="H50" s="93" t="str">
@@ -41027,11 +41025,11 @@
         <f>AU50-AV50</f>
         <v>0</v>
       </c>
-      <c r="BB50" s="112"/>
-      <c r="BC50" s="113"/>
-      <c r="BD50" s="113"/>
-      <c r="BE50" s="113"/>
-      <c r="BF50" s="114"/>
+      <c r="BB50" s="146"/>
+      <c r="BC50" s="147"/>
+      <c r="BD50" s="147"/>
+      <c r="BE50" s="147"/>
+      <c r="BF50" s="148"/>
     </row>
     <row r="51" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="23">
@@ -41053,8 +41051,12 @@
         <f>AB47</f>
         <v>England</v>
       </c>
-      <c r="F51" s="152"/>
-      <c r="G51" s="153"/>
+      <c r="F51" s="111">
+        <v>0</v>
+      </c>
+      <c r="G51" s="112">
+        <v>1</v>
+      </c>
       <c r="H51" s="93" t="str">
         <f>AB44</f>
         <v>Belgium</v>
@@ -41093,11 +41095,11 @@
       </c>
       <c r="S51" s="106" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>England_lose</v>
       </c>
       <c r="T51" s="106" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Belgium_win</v>
       </c>
       <c r="U51" s="102">
         <f t="shared" si="4"/>
@@ -41115,9 +41117,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y51" s="101" t="str">
+      <c r="Y51" s="101">
         <f t="shared" si="9"/>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AA51" s="101">
         <f>COUNTIF(AQ50:AQ53,CONCATENATE("&gt;=",AQ51))</f>
@@ -41211,11 +41213,11 @@
         <f>AU51-AV51</f>
         <v>0</v>
       </c>
-      <c r="BB51" s="112"/>
-      <c r="BC51" s="113"/>
-      <c r="BD51" s="113"/>
-      <c r="BE51" s="113"/>
-      <c r="BF51" s="114"/>
+      <c r="BB51" s="146"/>
+      <c r="BC51" s="147"/>
+      <c r="BD51" s="147"/>
+      <c r="BE51" s="147"/>
+      <c r="BF51" s="148"/>
     </row>
     <row r="52" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="23">
@@ -41237,8 +41239,12 @@
         <f>AB45</f>
         <v>Panama</v>
       </c>
-      <c r="F52" s="152"/>
-      <c r="G52" s="153"/>
+      <c r="F52" s="111">
+        <v>1</v>
+      </c>
+      <c r="G52" s="112">
+        <v>2</v>
+      </c>
       <c r="H52" s="93" t="str">
         <f>AB46</f>
         <v>Tunisia</v>
@@ -41277,11 +41283,11 @@
       </c>
       <c r="S52" s="106" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Panama_lose</v>
       </c>
       <c r="T52" s="106" t="str">
         <f t="shared" si="3"/>
-        <v/>
+        <v>Tunisia_win</v>
       </c>
       <c r="U52" s="102">
         <f t="shared" si="4"/>
@@ -41299,9 +41305,9 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Y52" s="101" t="str">
+      <c r="Y52" s="101">
         <f t="shared" si="9"/>
-        <v/>
+        <v>-1</v>
       </c>
       <c r="AA52" s="101">
         <f>COUNTIF(AQ50:AQ53,CONCATENATE("&gt;=",AQ52))</f>
@@ -41391,11 +41397,11 @@
         <f>AU52-AV52</f>
         <v>0</v>
       </c>
-      <c r="BB52" s="115"/>
-      <c r="BC52" s="116"/>
-      <c r="BD52" s="116"/>
-      <c r="BE52" s="116"/>
-      <c r="BF52" s="117"/>
+      <c r="BB52" s="149"/>
+      <c r="BC52" s="150"/>
+      <c r="BD52" s="150"/>
+      <c r="BE52" s="150"/>
+      <c r="BF52" s="151"/>
     </row>
     <row r="53" spans="1:58" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="23">
@@ -41417,10 +41423,10 @@
         <f>AB53</f>
         <v>Japan</v>
       </c>
-      <c r="F53" s="152">
-        <v>0</v>
-      </c>
-      <c r="G53" s="153">
+      <c r="F53" s="111">
+        <v>0</v>
+      </c>
+      <c r="G53" s="112">
         <v>1</v>
       </c>
       <c r="H53" s="93" t="str">
@@ -41596,10 +41602,10 @@
         <f>AB51</f>
         <v>Senegal</v>
       </c>
-      <c r="F54" s="154">
-        <v>0</v>
-      </c>
-      <c r="G54" s="155">
+      <c r="F54" s="113">
+        <v>0</v>
+      </c>
+      <c r="G54" s="114">
         <v>1</v>
       </c>
       <c r="H54" s="94" t="str">
@@ -42008,27 +42014,6 @@
   </sheetData>
   <sheetProtection algorithmName="SHA-512" hashValue="vGy7tfgNF+LQYUz/y1sllFN7upYEDbT6a7whpBRlO0wcZnEmOFaRTNIlFMR//q/21PrdL4BJIvFyIXko3KhKPA==" saltValue="6fdwo3QidqzBFmJPM6Ojlg==" spinCount="100000" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="28">
-    <mergeCell ref="BW6:CA7"/>
-    <mergeCell ref="A1:P1"/>
-    <mergeCell ref="O3:P3"/>
-    <mergeCell ref="A5:H6"/>
-    <mergeCell ref="J5:P6"/>
-    <mergeCell ref="BB10:BB11"/>
-    <mergeCell ref="BI12:BI13"/>
-    <mergeCell ref="BB6:BF7"/>
-    <mergeCell ref="BI6:BM7"/>
-    <mergeCell ref="BP6:BT7"/>
-    <mergeCell ref="BB22:BB23"/>
-    <mergeCell ref="BW23:BW24"/>
-    <mergeCell ref="BB18:BB19"/>
-    <mergeCell ref="BI20:BI21"/>
-    <mergeCell ref="BB14:BB15"/>
-    <mergeCell ref="BP16:BP17"/>
-    <mergeCell ref="BB30:BB31"/>
-    <mergeCell ref="BW31:CA32"/>
-    <mergeCell ref="BP32:BP33"/>
-    <mergeCell ref="BB26:BB27"/>
-    <mergeCell ref="BI28:BI29"/>
     <mergeCell ref="BB46:BF52"/>
     <mergeCell ref="BB38:BB39"/>
     <mergeCell ref="BO41:BT42"/>
@@ -42036,6 +42021,27 @@
     <mergeCell ref="BW35:BW36"/>
     <mergeCell ref="BI36:BI37"/>
     <mergeCell ref="BU41:CA42"/>
+    <mergeCell ref="BB30:BB31"/>
+    <mergeCell ref="BW31:CA32"/>
+    <mergeCell ref="BP32:BP33"/>
+    <mergeCell ref="BB26:BB27"/>
+    <mergeCell ref="BI28:BI29"/>
+    <mergeCell ref="BB22:BB23"/>
+    <mergeCell ref="BW23:BW24"/>
+    <mergeCell ref="BB18:BB19"/>
+    <mergeCell ref="BI20:BI21"/>
+    <mergeCell ref="BB14:BB15"/>
+    <mergeCell ref="BP16:BP17"/>
+    <mergeCell ref="BB10:BB11"/>
+    <mergeCell ref="BI12:BI13"/>
+    <mergeCell ref="BB6:BF7"/>
+    <mergeCell ref="BI6:BM7"/>
+    <mergeCell ref="BP6:BT7"/>
+    <mergeCell ref="BW6:CA7"/>
+    <mergeCell ref="A1:P1"/>
+    <mergeCell ref="O3:P3"/>
+    <mergeCell ref="A5:H6"/>
+    <mergeCell ref="J5:P6"/>
   </mergeCells>
   <conditionalFormatting sqref="F45:F55">
     <cfRule type="expression" dxfId="181" priority="120" stopIfTrue="1">

</xml_diff>